<commit_message>
New added script and Updated Commit = 29/09/2020
</commit_message>
<xml_diff>
--- a/rrd/AppData/Lead_Config_CriteriaLogic.xlsx
+++ b/rrd/AppData/Lead_Config_CriteriaLogic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA23430-C0AB-45D0-8665-CD109654EFF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FA24D1-D0F5-4517-AF9E-088136D534EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="13" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lead_Config16_CL" sheetId="13" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="24">
   <si>
     <t>RRD_Crieteria</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>afghanistan</t>
+  </si>
+  <si>
+    <t>Pratapgarh</t>
+  </si>
+  <si>
+    <t>Hydrabad</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DA9A96-2D33-4504-B71F-AC5A1989C338}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -640,7 +648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7870F20C-A9F5-4BB2-920E-AB5B53650D16}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -671,7 +681,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -731,7 +741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8CF1AB-D634-4141-BDE4-6B1D3A7A2850}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -775,7 +787,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D11A856-65DD-4FBD-9BC6-809A5C295B22}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -806,7 +820,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -817,6 +831,244 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4CB2FD9-1388-4B01-8D86-28DAC3014B03}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803CC19B-46E8-4276-8F7A-77B73E6748CA}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DED53CF-1D90-4AE0-A78B-A568EE81582B}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96A22C8-1F99-4AE3-A532-CAD8A1DE3B25}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA334AB-A30C-4259-AC50-0C144524CC87}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8357F0-2CB4-43DA-9BE6-2E0923AE53A9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -825,35 +1077,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
+    <col min="1" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>11</v>
@@ -864,151 +1115,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803CC19B-46E8-4276-8F7A-77B73E6748CA}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DED53CF-1D90-4AE0-A78B-A568EE81582B}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>500</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96A22C8-1F99-4AE3-A532-CAD8A1DE3B25}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>500</v>
-      </c>
-      <c r="D2" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA334AB-A30C-4259-AC50-0C144524CC87}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFB7B45-F2F9-4A65-8DD3-4505E2E6D79F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1039,100 +1147,6 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC8357F0-2CB4-43DA-9BE6-2E0923AE53A9}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFB7B45-F2F9-4A65-8DD3-4505E2E6D79F}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">

</xml_diff>